<commit_message>
Actualización archivo de lineas
</commit_message>
<xml_diff>
--- a/LineasMiCuentaWeb.xlsx
+++ b/LineasMiCuentaWeb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Telecom\WebPersonal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7B7A9D00-1442-4455-90C3-773B284FF7B6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B9960E79-212A-4E06-BFAD-441891F14F0A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,35 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="137">
-  <si>
-    <t>Mix</t>
-  </si>
-  <si>
-    <t>Pre</t>
-  </si>
-  <si>
-    <t>Pos</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>Linea</t>
   </si>
   <si>
-    <t>3758649203</t>
-  </si>
-  <si>
-    <t>transferencia de llamada POS</t>
-  </si>
-  <si>
-    <t>1162733281</t>
-  </si>
-  <si>
-    <t>3854041917</t>
-  </si>
-  <si>
-    <t>1164473518</t>
-  </si>
-  <si>
     <t>Caso</t>
   </si>
   <si>
@@ -283,9 +259,6 @@
   </si>
   <si>
     <t>DIGITAL_WEB_IND_FACTURACION_ADHESION_DEBITO_DIRECTO_MIX_CBU_INPUT_NUM_CARACT_MAX_Mas_de_22_digitos</t>
-  </si>
-  <si>
-    <t>input mail</t>
   </si>
   <si>
     <t>DIGITAL_WEB_IND_FACTURACION_ADHESION_DEBITO_DIRECTO_MIX_CBU_INPUT_NUM_CARACT_MAX_Menos_de_22_digitos</t>
@@ -527,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -537,8 +510,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="B127" sqref="B127"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,10 +804,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -851,9 +822,9 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="9">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
         <v>1164735148</v>
       </c>
       <c r="C2" s="1"/>
@@ -867,7 +838,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5">
         <v>1162745165</v>
@@ -883,7 +854,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B4" s="5">
         <v>1162735148</v>
@@ -899,7 +870,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5">
         <v>1162745165</v>
@@ -915,7 +886,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5">
         <v>1162735148</v>
@@ -931,7 +902,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>1162735148</v>
@@ -945,7 +916,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B8" s="5">
         <v>1162745165</v>
@@ -959,7 +930,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5">
         <v>1162735148</v>
@@ -973,7 +944,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B10" s="5">
         <v>1162745165</v>
@@ -989,7 +960,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B11" s="5">
         <v>1145642605</v>
@@ -1005,7 +976,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B12" s="5">
         <v>1145642605</v>
@@ -1021,7 +992,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B13" s="5">
         <v>1162745165</v>
@@ -1037,7 +1008,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B14" s="5">
         <v>1162735148</v>
@@ -1053,7 +1024,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B15" s="5">
         <v>1162745165</v>
@@ -1069,7 +1040,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B16" s="5">
         <v>1162735148</v>
@@ -1085,7 +1056,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B17" s="5">
         <v>1162745165</v>
@@ -1101,7 +1072,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B18" s="5">
         <v>1162735148</v>
@@ -1117,7 +1088,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B19" s="5">
         <v>1162745165</v>
@@ -1133,7 +1104,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B20" s="5">
         <v>1145642605</v>
@@ -1149,7 +1120,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B21" s="5">
         <v>1162735148</v>
@@ -1165,7 +1136,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B22" s="5">
         <v>1145642605</v>
@@ -1181,7 +1152,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B23" s="5">
         <v>1162745165</v>
@@ -1197,7 +1168,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B24" s="5">
         <v>1145642605</v>
@@ -1213,7 +1184,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B25" s="5">
         <v>1162735148</v>
@@ -1227,7 +1198,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B26" s="5">
         <v>1162735148</v>
@@ -1241,7 +1212,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B27" s="5">
         <v>1162745165</v>
@@ -1255,7 +1226,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B28" s="5">
         <v>1162735148</v>
@@ -1271,7 +1242,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B29" s="5">
         <v>1145642605</v>
@@ -1287,7 +1258,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B30" s="5">
         <v>1145642605</v>
@@ -1303,7 +1274,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B31" s="5">
         <v>1162735148</v>
@@ -1311,7 +1282,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B32" s="5">
         <v>1145642605</v>
@@ -1319,7 +1290,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B33" s="5">
         <v>1162735148</v>
@@ -1327,7 +1298,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B34" s="5">
         <v>1162745165</v>
@@ -1335,7 +1306,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B35" s="5">
         <v>1162735148</v>
@@ -1343,7 +1314,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B36" s="5">
         <v>1162745165</v>
@@ -1351,7 +1322,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B37" s="5">
         <v>1162735148</v>
@@ -1359,7 +1330,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B38" s="5">
         <v>1162745165</v>
@@ -1367,7 +1338,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B39" s="5">
         <v>1162735148</v>
@@ -1375,7 +1346,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B40" s="5">
         <v>1162735148</v>
@@ -1383,7 +1354,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B41" s="5">
         <v>1162745165</v>
@@ -1391,7 +1362,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B42" s="5">
         <v>1162735148</v>
@@ -1399,7 +1370,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B43" s="5">
         <v>1162735148</v>
@@ -1407,7 +1378,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B44" s="5">
         <v>1162735148</v>
@@ -1415,7 +1386,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B45" s="5">
         <v>1145642605</v>
@@ -1423,7 +1394,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B46" s="5">
         <v>1162735148</v>
@@ -1431,7 +1402,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B47" s="5">
         <v>1145642605</v>
@@ -1439,7 +1410,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B48" s="5">
         <v>1162745165</v>
@@ -1447,7 +1418,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B49" s="5">
         <v>1162735148</v>
@@ -1455,7 +1426,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B50" s="5">
         <v>1162745165</v>
@@ -1463,7 +1434,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B51" s="5">
         <v>1162735148</v>
@@ -1471,7 +1442,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B52" s="5">
         <v>1162735148</v>
@@ -1479,7 +1450,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B53" s="5">
         <v>1162735148</v>
@@ -1487,7 +1458,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B54" s="5">
         <v>1162735148</v>
@@ -1495,7 +1466,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B55" s="5">
         <v>1162735148</v>
@@ -1503,7 +1474,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B56" s="5">
         <v>1162735148</v>
@@ -1511,7 +1482,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B57" s="5">
         <v>1162735148</v>
@@ -1519,7 +1490,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B58" s="5">
         <v>1162735148</v>
@@ -1527,7 +1498,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B59" s="5">
         <v>1162735148</v>
@@ -1535,7 +1506,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B60" s="8">
         <v>3758649203</v>
@@ -1543,7 +1514,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B61" s="8">
         <v>3758649203</v>
@@ -1551,7 +1522,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B62" s="8">
         <v>3758649203</v>
@@ -1559,7 +1530,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B63" s="8">
         <v>3758649203</v>
@@ -1567,165 +1538,135 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B64" s="8">
         <v>3758649203</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B65" s="5">
         <v>1162735148</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B66" s="5">
         <v>1162735148</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D66" s="5">
-        <v>1162735148</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B67" s="8">
         <v>3758649203</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D67" s="5">
-        <v>1162745165</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B68" s="8">
         <v>3758649203</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D68" s="5">
-        <v>1145642605</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="5">
+        <v>1162735148</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="5">
+        <v>1162735148</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" s="5">
+        <v>1162735148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="5">
+        <v>1162735148</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" s="5">
+        <v>1162735148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" s="5">
+        <v>1162735148</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="5">
+        <v>1162735148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" s="5">
+        <v>1162735148</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>77</v>
-      </c>
-      <c r="B69" s="5">
-        <v>1162735148</v>
-      </c>
-      <c r="C69" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D69" s="8">
-        <v>3758649203</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>78</v>
-      </c>
-      <c r="B70" s="5">
-        <v>1162735148</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D70" s="5">
-        <v>1166248383</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>79</v>
-      </c>
-      <c r="B71" s="5">
-        <v>1162735148</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>80</v>
-      </c>
-      <c r="B72" s="5">
-        <v>1162735148</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>81</v>
-      </c>
-      <c r="B73" s="5">
-        <v>1162735148</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>82</v>
-      </c>
-      <c r="B74" s="5">
-        <v>1162735148</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>83</v>
-      </c>
-      <c r="B75" s="5">
-        <v>1162735148</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>84</v>
-      </c>
-      <c r="B76" s="5">
-        <v>1162735148</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>85</v>
       </c>
       <c r="B77" s="8">
         <v>3758649203</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B78" s="8">
         <v>3758649203</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B79" s="5">
         <v>1166248383</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B80" s="5">
         <v>1166248383</v>
@@ -1733,7 +1674,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B81" s="5">
         <v>3496652414</v>
@@ -1741,7 +1682,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B82" s="5">
         <v>3794601129</v>
@@ -1749,7 +1690,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B83" s="5">
         <v>1164520012</v>
@@ -1757,7 +1698,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B84" s="5">
         <v>1164461283</v>
@@ -1765,7 +1706,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B85" s="5">
         <v>1164480623</v>
@@ -1773,7 +1714,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B86" s="5">
         <v>1164461283</v>
@@ -1781,7 +1722,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B87" s="5">
         <v>1164480623</v>
@@ -1789,7 +1730,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B88" s="5">
         <v>1162755344</v>
@@ -1797,7 +1738,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B89" s="5">
         <v>1164405558</v>
@@ -1805,7 +1746,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B90" s="5">
         <v>1166248383</v>
@@ -1813,7 +1754,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B91" s="5">
         <v>1164493210</v>
@@ -1821,7 +1762,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B92" s="5">
         <v>1164493210</v>
@@ -1829,7 +1770,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B93" s="5">
         <v>1164493210</v>
@@ -1837,15 +1778,15 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>103</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>6</v>
+        <v>94</v>
+      </c>
+      <c r="B94" s="5">
+        <v>1162733281</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B95" s="5">
         <v>3413130145</v>
@@ -1853,15 +1794,15 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>105</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>6</v>
+        <v>96</v>
+      </c>
+      <c r="B96" s="5">
+        <v>1162733281</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B97" s="5">
         <v>1165990597</v>
@@ -1869,7 +1810,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B98" s="5">
         <v>1166248383</v>
@@ -1877,15 +1818,15 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>108</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>6</v>
+        <v>99</v>
+      </c>
+      <c r="B99" s="5">
+        <v>1162733281</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B100" s="5">
         <v>1166248383</v>
@@ -1893,15 +1834,15 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>110</v>
-      </c>
-      <c r="B101">
+        <v>101</v>
+      </c>
+      <c r="B101" s="8">
         <v>1162645152</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B102" s="5">
         <v>1161120234</v>
@@ -1909,39 +1850,39 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>112</v>
-      </c>
-      <c r="B103" s="6" t="s">
-        <v>4</v>
+        <v>103</v>
+      </c>
+      <c r="B103" s="6">
+        <v>3758649203</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>113</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>7</v>
+        <v>104</v>
+      </c>
+      <c r="B104" s="5">
+        <v>3854041917</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>114</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>8</v>
+        <v>105</v>
+      </c>
+      <c r="B105" s="5">
+        <v>1164473518</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>115</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>6</v>
+        <v>106</v>
+      </c>
+      <c r="B106" s="5">
+        <v>1162733281</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B107" s="5">
         <v>1165990597</v>
@@ -1949,7 +1890,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B108" s="5">
         <v>1162749941</v>
@@ -1957,7 +1898,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B109" s="5">
         <v>1145642605</v>
@@ -1965,7 +1906,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B110" s="5">
         <v>1162745165</v>
@@ -1973,7 +1914,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B111" s="5">
         <v>1164520012</v>
@@ -1981,7 +1922,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B112" s="8">
         <v>1152292615</v>
@@ -1989,7 +1930,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B113" s="5">
         <v>1164599468</v>
@@ -1997,7 +1938,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B114" s="5">
         <v>1164599450</v>
@@ -2005,7 +1946,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B115" s="5">
         <v>1162745165</v>
@@ -2013,15 +1954,15 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>125</v>
-      </c>
-      <c r="B116" s="5" t="s">
-        <v>6</v>
+        <v>116</v>
+      </c>
+      <c r="B116" s="5">
+        <v>1162733281</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B117" s="5">
         <v>1165990597</v>
@@ -2029,31 +1970,31 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>127</v>
-      </c>
-      <c r="B118" s="5" t="s">
-        <v>7</v>
+        <v>118</v>
+      </c>
+      <c r="B118" s="5">
+        <v>3854041917</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>128</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>8</v>
+        <v>119</v>
+      </c>
+      <c r="B119" s="5">
+        <v>1164473518</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>129</v>
-      </c>
-      <c r="B120">
+        <v>120</v>
+      </c>
+      <c r="B120" s="8">
         <v>1162816939</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B121" s="8">
         <v>3758649203</v>
@@ -2061,7 +2002,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B122" s="8">
         <v>3758649203</v>
@@ -2069,7 +2010,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B123" s="8">
         <v>3758649203</v>
@@ -2077,7 +2018,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B124" s="8">
         <v>3758649203</v>
@@ -2085,7 +2026,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B125" s="8">
         <v>3758649203</v>
@@ -2093,7 +2034,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B126" s="8">
         <v>3758649203</v>
@@ -2101,7 +2042,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B127" s="8">
         <v>3758649203</v>

</xml_diff>

<commit_message>
Nueva linea para caso headers
Nueva linea para caso headers
</commit_message>
<xml_diff>
--- a/LineasMiCuentaWeb.xlsx
+++ b/LineasMiCuentaWeb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A674155\eclipse-workspace\WebPersonal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Telecom\WebPersonal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2A7CC165-A8C3-4F3B-983D-D0A7A431D748}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B8F23459-B51F-4A34-9305-A130866DF9C3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t>Linea</t>
   </si>
@@ -409,6 +409,9 @@
   </si>
   <si>
     <t>DIGITAL_WEB_IND_FACTURACION_FACTURA_ONLINE_MIX_EMAIL_FORMATO_INVALIDO_sin_dato</t>
+  </si>
+  <si>
+    <t>Headers_Validar_links</t>
   </si>
 </sst>
 </file>
@@ -736,11 +739,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="130" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -1763,8 +1766,12 @@
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A128" s="1"/>
-      <c r="B128" s="1"/>
+      <c r="A128" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B128">
+        <v>1164473518</v>
+      </c>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>

</xml_diff>